<commit_message>
Combined weather data from tow sources.
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,42 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-10-31 12:39:51</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-10-31 12:42:59</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-10-31 12:47:45</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added error logging, but not implemented everywhere
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -673,6 +673,30 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-11-02 18:08:29</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-11-02 18:10:15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added email scheduling to weather bot
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -992,6 +992,58 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-11-04 11:01:41</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+    &lt;!DOCTYPE html&gt;
+    &lt;html lang="en"&gt;
+    &lt;head&gt;
+        &lt;meta charset="UTF-8"&gt;
+         &lt;style&gt;
+            body { font-family: Arial, sans-serif; margin: 20px; }
+            h1 { color: #333; }
+            h2 { color: #555; margin-top: 20px; }
+            table { width: 80%; border-collapse: collapse; margin-bottom: 20px; }
+            th, td { border: 1px solid #ddd; padding: 10px; text-align: left; }
+            th { background-color: #f2f2f2; color: #333; }
+            tr:nth-child(even) { background-color: #f9f9f9; }
+            tr:hover { background-color: #ddd; }
+            /* Specific styles for averages */
+            .averages-table {
+                width: 80%;
+                margin-top: 20px;
+                border: 2px solid #007BFF; /* blue border for emphasis */
+            }
+            .averages-table th {
+                background-color: #007BFF; /* blue background for headers */
+                color: white; /* white text for headers */
+                font-weight: bold;
+            }
+            .averages-table td {
+                background-color: #E7F1FF; /* light blue background for data */
+            }
+        &lt;/style&gt;
+    &lt;/head&gt;
+    &lt;body&gt;
+    &lt;h1&gt;Weather Report&lt;/h1&gt;
+    &lt;h2&gt;Averages:&lt;/h2&gt;
+    &lt;table class="averages-table"&gt;
+    &lt;tr&gt;
+    &lt;th&gt;Kaupunki&lt;/th&gt;&lt;th&gt;Keskimääräinen lämpötila&lt;/th&gt;&lt;th&gt;Keskimääräinen tuulen nopeus&lt;/th&gt;&lt;th&gt;Säätila&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Helsinki&lt;/td&gt;&lt;td&gt;1.7 Celsius&lt;/td&gt;&lt;td&gt;14.0 m/s&lt;/td&gt;&lt;td&gt;Ei merkittäviä sääilmiöitä&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Espoo&lt;/td&gt;&lt;td&gt;1.2 Celsius&lt;/td&gt;&lt;td&gt;9.3 m/s&lt;/td&gt;&lt;td&gt;Ei merkittäviä sääilmiöitä&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Vantaa&lt;/td&gt;&lt;td&gt;0.3 Celsius&lt;/td&gt;&lt;td&gt;9.9 m/s&lt;/td&gt;&lt;td&gt;Ei merkittäviä sääilmiöitä&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;h2&gt;Source: OpenWeatherMap&lt;/h2&gt;&lt;table border='1'&gt;&lt;tr&gt;&lt;th&gt;Kaupunki&lt;/th&gt;&lt;th&gt;Lämpötila&lt;/th&gt;&lt;th&gt;Säätila&lt;/th&gt;&lt;th&gt;Tuulen_nopeus&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Helsinki&lt;/td&gt;&lt;td&gt;1.12&lt;/td&gt;&lt;td&gt;moderate rain&lt;/td&gt;&lt;td&gt;8.05&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Espoo&lt;/td&gt;&lt;td&gt;0.8&lt;/td&gt;&lt;td&gt;moderate rain&lt;/td&gt;&lt;td&gt;5.14&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Vantaa&lt;/td&gt;&lt;td&gt;0.67&lt;/td&gt;&lt;td&gt;moderate rain&lt;/td&gt;&lt;td&gt;5.14&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;h2&gt;Source: Finnish Meteorological Institute&lt;/h2&gt;&lt;table border='1'&gt;&lt;tr&gt;&lt;th&gt;Kaupunki&lt;/th&gt;&lt;th&gt;Lämpötila&lt;/th&gt;&lt;th&gt;Säätila&lt;/th&gt;&lt;th&gt;Tuulen_nopeus&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Helsinki&lt;/td&gt;&lt;td&gt;2.2 Celsius&lt;/td&gt;&lt;td&gt;Ei merkittäviä sääilmiöitä&lt;/td&gt;&lt;td&gt;5.9 m/s avarage speed measured in the last 10 minutes&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Espoo&lt;/td&gt;&lt;td&gt;1.7 Celsius&lt;/td&gt;&lt;td&gt;Ei merkittäviä sääilmiöitä&lt;/td&gt;&lt;td&gt;4.2 m/s avarage speed measured in the last 10 minutes&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Vantaa&lt;/td&gt;&lt;td&gt;-0.1 Celsius&lt;/td&gt;&lt;td&gt;Ei merkittäviä sääilmiöitä&lt;/td&gt;&lt;td&gt;4.8 m/s avarage speed measured in the last 10 minutes&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;&lt;/body&gt;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
error situation handling is better in dataHandling.py
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -1051,6 +1051,65 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-11-04 10:44:40</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+    &lt;!DOCTYPE html&gt;
+    &lt;html&gt;
+    &lt;head&gt;
+        &lt;style&gt;
+            table {
+                font-family: Arial, sans-serif;
+                border-collapse: collapse;
+                width: 100%;
+            }
+            th, td {
+                border: 1px solid #dddddd;
+                text-align: left;
+                padding: 8px;
+            }
+            th {
+                background-color: #f2f2f2;
+            }
+        &lt;/style&gt;
+    &lt;/head&gt;
+    &lt;body&gt;
+    &lt;h2&gt;Error Log&lt;/h2&gt;
+    &lt;table&gt;
+        &lt;tr&gt;
+            &lt;th&gt;Timestamp&lt;/th&gt;
+            &lt;td&gt;2024-11-04 10:44:36&lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr&gt;
+            &lt;th&gt;Error Level&lt;/th&gt;
+            &lt;td&gt;High&lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr&gt;
+            &lt;th&gt;Location&lt;/th&gt;
+            &lt;td&gt;tasks.py, line 22&lt;/td&gt;
+        &lt;/tr&gt;
+        &lt;tr&gt;
+            &lt;th&gt;Error Message&lt;/th&gt;
+            &lt;td&gt;Testing!!!&lt;/td&gt;
+        &lt;/tr&gt;
+    &lt;/table&gt;
+    &lt;/body&gt;
+    &lt;/html&gt;
+    </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>